<commit_message>
Get results on valid splits
</commit_message>
<xml_diff>
--- a/experiments/hybrid/train.0.010/2-gram-weights.xlsx
+++ b/experiments/hybrid/train.0.010/2-gram-weights.xlsx
@@ -449,27 +449,27 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>('pretty', 'woman')</t>
+          <t>('looks', 'like')</t>
         </is>
       </c>
       <c r="B2" t="n">
         <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0396600566572238</v>
+        <v>0.03526448362720403</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>('low', 'budget')</t>
+          <t>('year', 'old')</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="n">
-        <v>0.0339943342776204</v>
+        <v>0.02770780856423174</v>
       </c>
     </row>
     <row r="4">
@@ -479,803 +479,803 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0339943342776204</v>
+        <v>0.02518891687657431</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>('bad', 'movie')</t>
+          <t>('really', 'bad')</t>
         </is>
       </c>
       <c r="B5" t="n">
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.028328611898017</v>
+        <v>0.02518891687657431</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>('mst', 'k')</t>
+          <t>('bad', 'acting')</t>
         </is>
       </c>
       <c r="B6" t="n">
         <v>10</v>
       </c>
       <c r="C6" t="n">
-        <v>0.028328611898017</v>
+        <v>0.02518891687657431</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>('whole', 'thing')</t>
+          <t>('one', 'worst')</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="n">
-        <v>0.028328611898017</v>
+        <v>0.02267002518891688</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>('camera', 'work')</t>
+          <t>('even', 'worse')</t>
         </is>
       </c>
       <c r="B8" t="n">
         <v>9</v>
       </c>
       <c r="C8" t="n">
-        <v>0.0254957507082153</v>
+        <v>0.02267002518891688</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'ever')</t>
+          <t>('stay', 'away')</t>
         </is>
       </c>
       <c r="B9" t="n">
         <v>9</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0254957507082153</v>
+        <v>0.02267002518891688</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>('dick', 'jane')</t>
+          <t>('movie', 'ever')</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0226628895184136</v>
+        <v>0.02267002518891688</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>('pretty', 'much')</t>
+          <t>('movie', 'see')</t>
         </is>
       </c>
       <c r="B11" t="n">
         <v>8</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0226628895184136</v>
+        <v>0.02015113350125945</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'would')</t>
+          <t>('movies', 'like')</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0198300283286119</v>
+        <v>0.02015113350125945</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>('really', 'really')</t>
+          <t>('tv', 'series')</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C13" t="n">
-        <v>0.0198300283286119</v>
+        <v>0.02015113350125945</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>('main', 'character')</t>
+          <t>('horror', 'movie')</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C14" t="n">
-        <v>0.0169971671388102</v>
+        <v>0.02015113350125945</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>('r', 'rated')</t>
+          <t>('movie', 'would')</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C15" t="n">
-        <v>0.0169971671388102</v>
+        <v>0.02015113350125945</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>('look', 'like')</t>
+          <t>('worth', 'watching')</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" t="n">
-        <v>0.0169971671388102</v>
+        <v>0.01763224181360202</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>('really', 'bad')</t>
+          <t>('high', 'school')</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C17" t="n">
-        <v>0.0169971671388102</v>
+        <v>0.01763224181360202</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>('one', 'would')</t>
+          <t>('even', 'get')</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18" t="n">
-        <v>0.0169971671388102</v>
+        <v>0.01763224181360202</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>('great', 'movie')</t>
+          <t>('seems', 'like')</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C19" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01763224181360202</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>('horror', 'film')</t>
+          <t>('like', 'movie')</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C20" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01763224181360202</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>('felt', 'like')</t>
+          <t>('like', 'one')</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C21" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01763224181360202</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>('film', 'like')</t>
+          <t>('movie', 'also')</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C22" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>('first', 'one')</t>
+          <t>('movie', 'could')</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C23" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'bad')</t>
+          <t>('worst', 'movie')</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C24" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>('worst', 'movie')</t>
+          <t>('movie', 'one')</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C25" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>('character', 'development')</t>
+          <t>('movie', 'first')</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C26" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>('rishi', 'kapoor')</t>
+          <t>('would', 'better')</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C27" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>('film', 'without')</t>
+          <t>('first', 'movie')</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C28" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>('first', 'half')</t>
+          <t>('sounds', 'like')</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C29" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>('waste', 'money')</t>
+          <t>('bad', 'one')</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C30" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>('sex', 'scenes')</t>
+          <t>('movie', 'think')</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C31" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'still')</t>
+          <t>('bad', 'movie')</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C32" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>('whole', 'movie')</t>
+          <t>('movie', 'bad')</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C33" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01511335012594458</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'even')</t>
+          <t>('martial', 'arts')</t>
         </is>
       </c>
       <c r="B34" t="n">
         <v>5</v>
       </c>
       <c r="C34" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>('happen', 'film')</t>
+          <t>('writer', 'director')</t>
         </is>
       </c>
       <c r="B35" t="n">
         <v>5</v>
       </c>
       <c r="C35" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>('see', 'dick')</t>
+          <t>('movie', 'makes')</t>
         </is>
       </c>
       <c r="B36" t="n">
         <v>5</v>
       </c>
       <c r="C36" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>('shahrukh', 'khan')</t>
+          <t>('watching', 'movie')</t>
         </is>
       </c>
       <c r="B37" t="n">
         <v>5</v>
       </c>
       <c r="C37" t="n">
-        <v>0.0141643059490085</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>('bu', 'uel')</t>
+          <t>('film', 'making')</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C38" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>('never', 'get')</t>
+          <t>('get', 'wrong')</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C39" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>('first', 'movie')</t>
+          <t>('bad', 'bad')</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C40" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>('want', 'watch')</t>
+          <t>('look', 'like')</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C41" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>('pretty', 'bad')</t>
+          <t>('movie', 'even')</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C42" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>('half', 'hour')</t>
+          <t>('movie', 'like')</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C43" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>('minutes', 'movie')</t>
+          <t>('slow', 'moving')</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C44" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>('looked', 'like')</t>
+          <t>('horror', 'films')</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C45" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>('yet', 'another')</t>
+          <t>('seen', 'film')</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C46" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>('hedy', 'lamarr')</t>
+          <t>('entire', 'film')</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C47" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>('could', 'good')</t>
+          <t>('never', 'seen')</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C48" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>('still', 'think')</t>
+          <t>('anyone', 'else')</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C49" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>('science', 'fiction')</t>
+          <t>('plot', 'line')</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C50" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>('awful', 'movie')</t>
+          <t>('pretty', 'bad')</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C51" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>('say', 'film')</t>
+          <t>('five', 'minutes')</t>
         </is>
       </c>
       <c r="B52" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C52" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>('original', 'film')</t>
+          <t>('many', 'times')</t>
         </is>
       </c>
       <c r="B53" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C53" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>('still', 'like')</t>
+          <t>('rest', 'movie')</t>
         </is>
       </c>
       <c r="B54" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C54" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>('good', 'enough')</t>
+          <t>('rest', 'cast')</t>
         </is>
       </c>
       <c r="B55" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C55" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>('like', 'could')</t>
+          <t>('none', 'characters')</t>
         </is>
       </c>
       <c r="B56" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C56" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>('year', 'olds')</t>
+          <t>('mst', 'k')</t>
         </is>
       </c>
       <c r="B57" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C57" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01259445843828715</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>('every', 'time')</t>
+          <t>('bad', 'movies')</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>4</v>
       </c>
       <c r="C58" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>('say', 'movie')</t>
+          <t>('little', 'boy')</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>4</v>
       </c>
       <c r="C59" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>('mary', 'lou')</t>
+          <t>('say', 'something')</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>('bad', 'acting')</t>
+          <t>('film', 'even')</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>4</v>
       </c>
       <c r="C61" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'almost')</t>
+          <t>('movie', 'horrible')</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>4</v>
       </c>
       <c r="C62" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>('many', 'people')</t>
+          <t>('time', 'money')</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>4</v>
       </c>
       <c r="C63" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>('watching', 'movie')</t>
+          <t>('george', 'mildred')</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>4</v>
       </c>
       <c r="C64" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>('really', 'think')</t>
+          <t>('characters', 'movie')</t>
         </is>
       </c>
       <c r="B65" t="n">
         <v>4</v>
       </c>
       <c r="C65" t="n">
-        <v>0.0113314447592068</v>
+        <v>0.01007556675062972</v>
       </c>
     </row>
   </sheetData>
@@ -1312,833 +1312,833 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>('tony', 'hawk')</t>
+          <t>('new', 'york')</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>35</v>
+        <v>12</v>
       </c>
       <c r="C2" t="n">
-        <v>0.0831353919239905</v>
+        <v>0.03934426229508197</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>('pro', 'skater')</t>
+          <t>('film', 'also')</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C3" t="n">
-        <v>0.05225653206650831</v>
+        <v>0.02950819672131148</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>('hawk', 'pro')</t>
+          <t>('pretty', 'good')</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="C4" t="n">
-        <v>0.05225653206650831</v>
+        <v>0.02950819672131148</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>('skater', 'x')</t>
+          <t>('movie', 'made')</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="C5" t="n">
-        <v>0.04513064133016627</v>
+        <v>0.02622950819672131</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>('one', 'best')</t>
+          <t>('rob', 'roy')</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="C6" t="n">
-        <v>0.04038004750593824</v>
+        <v>0.02622950819672131</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>('one', 'thing')</t>
+          <t>('quite', 'good')</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C7" t="n">
-        <v>0.02612826603325416</v>
+        <v>0.02295081967213115</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>('see', 'movie')</t>
+          <t>('young', 'man')</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C8" t="n">
-        <v>0.02137767220902613</v>
+        <v>0.01967213114754099</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>('first', 'time')</t>
+          <t>('one', 'people')</t>
         </is>
       </c>
       <c r="B9" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C9" t="n">
-        <v>0.01900237529691211</v>
+        <v>0.01967213114754099</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>('james', 'bond')</t>
+          <t>('anna', 'christie')</t>
         </is>
       </c>
       <c r="B10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0166270783847981</v>
+        <v>0.01967213114754099</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>('great', 'job')</t>
+          <t>('black', 'white')</t>
         </is>
       </c>
       <c r="B11" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C11" t="n">
-        <v>0.0166270783847981</v>
+        <v>0.01967213114754099</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>('first', 'film')</t>
+          <t>('well', 'done')</t>
         </is>
       </c>
       <c r="B12" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C12" t="n">
-        <v>0.0166270783847981</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>('say', 'never')</t>
+          <t>('good', 'film')</t>
         </is>
       </c>
       <c r="B13" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C13" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>('highly', 'recommend')</t>
+          <t>('would', 'like')</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C14" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>('chipmunk', 'adventure')</t>
+          <t>('great', 'deal')</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>('never', 'say')</t>
+          <t>('great', 'film')</t>
         </is>
       </c>
       <c r="B16" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C16" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'made')</t>
+          <t>('uncle', 'philip')</t>
         </is>
       </c>
       <c r="B17" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C17" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>('x', 'career')</t>
+          <t>('worth', 'seeing')</t>
         </is>
       </c>
       <c r="B18" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>('black', 'white')</t>
+          <t>('film', 'noir')</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>('ghost', 'stories')</t>
+          <t>('bug', 'life')</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C20" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>('get', 'see')</t>
+          <t>('melting', 'man')</t>
         </is>
       </c>
       <c r="B21" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>('first', 'saw')</t>
+          <t>('one', 'day')</t>
         </is>
       </c>
       <c r="B22" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C22" t="n">
-        <v>0.01425178147268409</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>('takes', 'place')</t>
+          <t>('movie', 'without')</t>
         </is>
       </c>
       <c r="B23" t="n">
         <v>5</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>('movie', 'good')</t>
+          <t>('real', 'life')</t>
         </is>
       </c>
       <c r="B24" t="n">
         <v>5</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01639344262295082</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>('like', 'one')</t>
+          <t>('well', 'worth')</t>
         </is>
       </c>
       <c r="B25" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>('well', 'made')</t>
+          <t>('two', 'films')</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>('subject', 'matter')</t>
+          <t>('feel', 'like')</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>('films', 'ever')</t>
+          <t>('get', 'together')</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>('never', 'seen')</t>
+          <t>('takes', 'place')</t>
         </is>
       </c>
       <c r="B29" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>('feel', 'like')</t>
+          <t>('several', 'times')</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>('bobby', 'earl')</t>
+          <t>('lion', 'king')</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>('main', 'characters')</t>
+          <t>('well', 'acted')</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>('never', 'heard')</t>
+          <t>('well', 'written')</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>('old', 'man')</t>
+          <t>('end', 'well')</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>('world', 'war')</t>
+          <t>('one', 'liners')</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>('anything', 'else')</t>
+          <t>('well', 'made')</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>('film', 'made')</t>
+          <t>('car', 'chases')</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C37" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>('game', 'play')</t>
+          <t>('two', 'years')</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>('movies', 'ever')</t>
+          <t>('many', 'ways')</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>('hawk', 'career')</t>
+          <t>('b', 'movie')</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C40" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>('one', 'film')</t>
+          <t>('film', 'festival')</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C41" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>('best', 'friend')</t>
+          <t>('muppet', 'movie')</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C42" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>('must', 'see')</t>
+          <t>('le', 'million')</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
-          <t>('gene', 'kelly')</t>
+          <t>('would', 'never')</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C44" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="1" t="inlineStr">
         <is>
-          <t>('one', 'night')</t>
+          <t>('never', 'get')</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C45" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="1" t="inlineStr">
         <is>
-          <t>('star', 'trek')</t>
+          <t>('hit', 'man')</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C46" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="1" t="inlineStr">
         <is>
-          <t>('second', 'time')</t>
+          <t>('never', 'made')</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C47" t="n">
-        <v>0.01187648456057007</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="1" t="inlineStr">
         <is>
-          <t>('like', 'really')</t>
+          <t>('art', 'action')</t>
         </is>
       </c>
       <c r="B48" t="n">
         <v>4</v>
       </c>
       <c r="C48" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="1" t="inlineStr">
         <is>
-          <t>('phantom', 'lady')</t>
+          <t>('beauty', 'art')</t>
         </is>
       </c>
       <c r="B49" t="n">
         <v>4</v>
       </c>
       <c r="C49" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="1" t="inlineStr">
         <is>
-          <t>('seen', 'movie')</t>
+          <t>('stan', 'ollie')</t>
         </is>
       </c>
       <c r="B50" t="n">
         <v>4</v>
       </c>
       <c r="C50" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="1" t="inlineStr">
         <is>
-          <t>('like', 'see')</t>
+          <t>('one', 'would')</t>
         </is>
       </c>
       <c r="B51" t="n">
         <v>4</v>
       </c>
       <c r="C51" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="1" t="inlineStr">
         <is>
-          <t>('beginning', 'end')</t>
+          <t>('film', 'really')</t>
         </is>
       </c>
       <c r="B52" t="n">
         <v>4</v>
       </c>
       <c r="C52" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="1" t="inlineStr">
         <is>
-          <t>('wagon', 'master')</t>
+          <t>('gives', 'film')</t>
         </is>
       </c>
       <c r="B53" t="n">
         <v>4</v>
       </c>
       <c r="C53" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="1" t="inlineStr">
         <is>
-          <t>('really', 'enjoyed')</t>
+          <t>('people', 'enjoy')</t>
         </is>
       </c>
       <c r="B54" t="n">
         <v>4</v>
       </c>
       <c r="C54" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="1" t="inlineStr">
         <is>
-          <t>('well', 'worth')</t>
+          <t>('good', 'little')</t>
         </is>
       </c>
       <c r="B55" t="n">
         <v>4</v>
       </c>
       <c r="C55" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="1" t="inlineStr">
         <is>
-          <t>('great', 'work')</t>
+          <t>('one', 'favorite')</t>
         </is>
       </c>
       <c r="B56" t="n">
         <v>4</v>
       </c>
       <c r="C56" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="1" t="inlineStr">
         <is>
-          <t>('young', 'woman')</t>
+          <t>('story', 'great')</t>
         </is>
       </c>
       <c r="B57" t="n">
         <v>4</v>
       </c>
       <c r="C57" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="1" t="inlineStr">
         <is>
-          <t>('old', 'fashioned')</t>
+          <t>('production', 'values')</t>
         </is>
       </c>
       <c r="B58" t="n">
         <v>4</v>
       </c>
       <c r="C58" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="1" t="inlineStr">
         <is>
-          <t>('action', 'films')</t>
+          <t>('little', 'film')</t>
         </is>
       </c>
       <c r="B59" t="n">
         <v>4</v>
       </c>
       <c r="C59" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="1" t="inlineStr">
         <is>
-          <t>('least', 'one')</t>
+          <t>('without', 'doubt')</t>
         </is>
       </c>
       <c r="B60" t="n">
         <v>4</v>
       </c>
       <c r="C60" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="1" t="inlineStr">
         <is>
-          <t>('gave', 'us')</t>
+          <t>('years', 'later')</t>
         </is>
       </c>
       <c r="B61" t="n">
         <v>4</v>
       </c>
       <c r="C61" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" s="1" t="inlineStr">
         <is>
-          <t>('works', 'well')</t>
+          <t>('must', 'see')</t>
         </is>
       </c>
       <c r="B62" t="n">
         <v>4</v>
       </c>
       <c r="C62" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" s="1" t="inlineStr">
         <is>
-          <t>('jack', 'frost')</t>
+          <t>('saw', 'movie')</t>
         </is>
       </c>
       <c r="B63" t="n">
         <v>4</v>
       </c>
       <c r="C63" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" s="1" t="inlineStr">
         <is>
-          <t>('bad', 'guys')</t>
+          <t>('york', 'love')</t>
         </is>
       </c>
       <c r="B64" t="n">
         <v>4</v>
       </c>
       <c r="C64" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.01311475409836066</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="1" t="inlineStr">
         <is>
-          <t>('wife', 'daughter')</t>
+          <t>('like', 'tv')</t>
         </is>
       </c>
       <c r="B65" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C65" t="n">
-        <v>0.009501187648456057</v>
+        <v>0.009836065573770493</v>
       </c>
     </row>
   </sheetData>

</xml_diff>